<commit_message>
add cell var callback
</commit_message>
<xml_diff>
--- a/tests/template-excel/sample-mix-output.xlsx
+++ b/tests/template-excel/sample-mix-output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Tim's grades</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Teacher Z</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>i was red color</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -76,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -96,6 +108,15 @@
       <name val="等线"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+    </font>
+    <font>
       <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
@@ -104,13 +125,34 @@
       <color rgb="FF000000"/>
       <name val="等线"/>
     </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -135,14 +177,26 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +497,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,11 +513,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customHeight="1" ht="23.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="1"/>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -471,10 +525,10 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
         <v>4</v>
@@ -548,7 +602,7 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="11">
         <v>85</v>
       </c>
       <c r="I6" s="1"/>
@@ -593,11 +647,11 @@
       <c r="K9"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="D10"/>
       <c r="E10" s="2" t="s">
         <v>14</v>
@@ -605,7 +659,7 @@
       <c r="F10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H10" t="s">
@@ -616,9 +670,9 @@
       <c r="K10"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
@@ -628,9 +682,9 @@
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -638,6 +692,52 @@
       <c r="I12" s="1"/>
       <c r="J12"/>
       <c r="K12"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16"/>
+      <c r="K16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>